<commit_message>
Fix for new web page
</commit_message>
<xml_diff>
--- a/Templates/CompanyList.xlsx
+++ b/Templates/CompanyList.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>會員編號</t>
   </si>
@@ -61,6 +61,15 @@
   </si>
   <si>
     <t>公司名稱</t>
+  </si>
+  <si>
+    <t>郵遞區號</t>
+  </si>
+  <si>
+    <t>相關資料</t>
+  </si>
+  <si>
+    <t>聯絡手機</t>
   </si>
 </sst>
 </file>
@@ -378,25 +387,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N1"/>
+  <dimension ref="A1:Q1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.5703125" customWidth="1"/>
-    <col min="3" max="7" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="13" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.5703125" customWidth="1"/>
+    <col min="3" max="5" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.5703125" customWidth="1"/>
+    <col min="7" max="8" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="15" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -413,31 +424,40 @@
         <v>3</v>
       </c>
       <c r="F1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>8</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>9</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
         <v>10</v>
       </c>
-      <c r="M1" t="s">
+      <c r="O1" t="s">
         <v>11</v>
       </c>
-      <c r="N1" t="s">
+      <c r="P1" t="s">
         <v>12</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>